<commit_message>
cleaned up some unused code and some restructuring
</commit_message>
<xml_diff>
--- a/excel_files/settings.xlsx
+++ b/excel_files/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tord\projects\macro\code\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCC0C99-90D5-4C33-8F6B-117F18E01A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9564DF2-5D2C-44D4-A1D1-E9DB627E636A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-8520" yWindow="-17560" windowWidth="18050" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>F</t>
   </si>
@@ -115,15 +115,6 @@
     <t>CCON, CWSR, COFF</t>
   </si>
   <si>
-    <t>Year of analysis:</t>
-  </si>
-  <si>
-    <t>History mode</t>
-  </si>
-  <si>
-    <t>On</t>
-  </si>
-  <si>
     <t>C_TWAS, C_TWAI, C_TAIR, CHEA, Waste</t>
   </si>
   <si>
@@ -131,6 +122,9 @@
   </si>
   <si>
     <t>R, S</t>
+  </si>
+  <si>
+    <t>YoA</t>
   </si>
 </sst>
 </file>
@@ -525,7 +519,7 @@
   <dimension ref="C1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10" x14ac:dyDescent="0.2"/>
@@ -544,11 +538,9 @@
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="3:6" x14ac:dyDescent="0.2">
@@ -558,9 +550,7 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2">
         <v>2017</v>
       </c>
@@ -651,16 +641,16 @@
         <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E13" s="1"/>
     </row>

</xml_diff>